<commit_message>
added Network Connectivity and Modified Device Stability
</commit_message>
<xml_diff>
--- a/src/test/resources/documents/XP5S_All_TC.xlsx
+++ b/src/test/resources/documents/XP5S_All_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="656" firstSheet="12" activeTab="12"/>
+    <workbookView windowWidth="20385" windowHeight="7935" tabRatio="656" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,12 @@
     <sheet name="XP5S_SonimCare" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <oleSize ref="A464:F514"/>
+  <oleSize ref="A443:F493"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096">
   <si>
     <t>Sonimcare</t>
   </si>
@@ -5412,6 +5412,18 @@
   </si>
   <si>
     <t>XP8_TC_003_Stability_Validate_MT_SMS</t>
+  </si>
+  <si>
+    <t>XP8_TC_001_Stability_Enable_Disable_MobileData_DeviceSettings</t>
+  </si>
+  <si>
+    <t>XP8_TC_002_Stability_Enable_Disable_Connection_Secured_Wifi_DeviceSettings</t>
+  </si>
+  <si>
+    <t>XP8_TC_003_Stability_Enable_Disable_Airplane_Devicesettings</t>
+  </si>
+  <si>
+    <t>XP8_TC_004_Stability_Enable_Disable_BT_And_Scan_BT_Devices</t>
   </si>
   <si>
     <t>XP8_TC_01_Stability_Setting_Up_Preconditions_Email</t>
@@ -6334,10 +6346,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -6416,11 +6428,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6447,9 +6465,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6462,6 +6479,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -6477,37 +6526,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -6517,21 +6535,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6612,7 +6624,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6624,13 +6726,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6648,97 +6786,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6750,43 +6798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6899,8 +6911,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6930,21 +6942,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -6962,8 +6959,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6983,6 +6980,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -6996,148 +7008,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -28110,10 +28122,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AY475"/>
+  <dimension ref="A1:AY491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
-      <selection activeCell="D269" sqref="D269"/>
+    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
+      <selection activeCell="F478" sqref="F478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -33009,8 +33021,126 @@
       <c r="I475" s="12"/>
       <c r="J475" s="19"/>
     </row>
+    <row r="477" s="7" customFormat="1" spans="1:4">
+      <c r="A477" s="48" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B477" s="48"/>
+      <c r="C477" s="48"/>
+      <c r="D477" s="48"/>
+    </row>
+    <row r="478" s="7" customFormat="1" spans="1:4">
+      <c r="A478" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B478" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="C478" s="49" t="s">
+        <v>517</v>
+      </c>
+      <c r="D478" s="49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="479" s="7" customFormat="1" spans="1:4">
+      <c r="A479" s="26">
+        <v>1</v>
+      </c>
+      <c r="B479" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="C479" s="149" t="s">
+        <v>523</v>
+      </c>
+      <c r="D479" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="480" s="7" customFormat="1"/>
+    <row r="481" s="7" customFormat="1" spans="1:3">
+      <c r="A481" s="9" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B481" s="9"/>
+      <c r="C481" s="9"/>
+    </row>
+    <row r="482" s="7" customFormat="1" spans="1:3">
+      <c r="A482" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B482" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="C482" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="483" s="7" customFormat="1" spans="1:3">
+      <c r="A483" s="11">
+        <v>1</v>
+      </c>
+      <c r="B483" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="C483" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="484" s="7" customFormat="1"/>
+    <row r="485" s="7" customFormat="1" spans="1:3">
+      <c r="A485" s="9" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B485" s="9"/>
+      <c r="C485" s="9"/>
+    </row>
+    <row r="486" s="7" customFormat="1" spans="1:3">
+      <c r="A486" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B486" s="28"/>
+      <c r="C486" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="487" s="7" customFormat="1" spans="1:3">
+      <c r="A487" s="11">
+        <v>1</v>
+      </c>
+      <c r="B487" s="50"/>
+      <c r="C487" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="488" s="7" customFormat="1"/>
+    <row r="489" s="7" customFormat="1" spans="1:3">
+      <c r="A489" s="9" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B489" s="9"/>
+      <c r="C489" s="9"/>
+    </row>
+    <row r="490" s="7" customFormat="1" spans="1:3">
+      <c r="A490" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B490" s="28"/>
+      <c r="C490" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="491" s="7" customFormat="1" spans="1:3">
+      <c r="A491" s="11">
+        <v>1</v>
+      </c>
+      <c r="B491" s="50"/>
+      <c r="C491" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="119">
+  <mergeCells count="123">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A9:C9"/>
@@ -33130,6 +33260,10 @@
     <mergeCell ref="A465:C465"/>
     <mergeCell ref="A469:J469"/>
     <mergeCell ref="A473:J473"/>
+    <mergeCell ref="A477:D477"/>
+    <mergeCell ref="A481:C481"/>
+    <mergeCell ref="A485:C485"/>
+    <mergeCell ref="A489:C489"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1" display="www.google.co.in"/>
@@ -33176,6 +33310,8 @@
     <hyperlink ref="B259" r:id="rId17" display="www.dtdc.com" tooltip="http://www.dtdc.com"/>
     <hyperlink ref="D263" r:id="rId25" display="sanity.test.sonim@gmail.com"/>
     <hyperlink ref="E263" r:id="rId26" display="password@12345" tooltip="mailto:password@12345"/>
+    <hyperlink ref="B479" r:id="rId1" display="www.google.co.in"/>
+    <hyperlink ref="B483" r:id="rId1" display="www.google.co.in"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -33328,7 +33464,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="9" t="s">
-        <v>1790</v>
+        <v>1794</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -33349,16 +33485,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>1791</v>
+        <v>1795</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>1792</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="9" t="s">
-        <v>1793</v>
+        <v>1797</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -33380,7 +33516,7 @@
         <v>1477</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>1794</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="75" spans="1:6">
@@ -33391,22 +33527,22 @@
         <v>1479</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>1795</v>
+        <v>1799</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>1796</v>
+        <v>1800</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>1797</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="9" t="s">
-        <v>1798</v>
+        <v>1802</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -33428,7 +33564,7 @@
         <v>1477</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>1794</v>
+        <v>1798</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>1210</v>
@@ -33442,25 +33578,25 @@
         <v>1479</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>1795</v>
+        <v>1799</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>1799</v>
+        <v>1803</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>1800</v>
+        <v>1804</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>1801</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="9" t="s">
-        <v>1802</v>
+        <v>1806</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -33490,19 +33626,19 @@
         <v>1479</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>1795</v>
+        <v>1799</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>1803</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="9" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -33524,13 +33660,13 @@
         <v>570</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>1805</v>
+        <v>1809</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>529</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>1806</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -33538,31 +33674,31 @@
         <v>1</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>1807</v>
+        <v>1811</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>573</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>1808</v>
+        <v>1812</v>
       </c>
       <c r="E35" s="45" t="s">
         <v>1071</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>1809</v>
+        <v>1813</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>530</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>1810</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="9" t="s">
-        <v>1811</v>
+        <v>1815</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -33649,7 +33785,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>1812</v>
+        <v>1816</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -33679,7 +33815,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="35" t="s">
-        <v>1813</v>
+        <v>1817</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -33709,7 +33845,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="35" t="s">
-        <v>1814</v>
+        <v>1818</v>
       </c>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -33739,7 +33875,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:8">
       <c r="A13" s="36" t="s">
-        <v>1815</v>
+        <v>1819</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>
@@ -33804,7 +33940,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="35" t="s">
-        <v>1816</v>
+        <v>1820</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -33834,7 +33970,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="35" t="s">
-        <v>1817</v>
+        <v>1821</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -33864,7 +34000,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:4">
       <c r="A25" s="39" t="s">
-        <v>1818</v>
+        <v>1822</v>
       </c>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -33906,7 +34042,7 @@
     </row>
     <row r="29" customFormat="1" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>1819</v>
+        <v>1823</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -33939,7 +34075,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>1820</v>
+        <v>1824</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -33969,7 +34105,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>1821</v>
+        <v>1825</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -33999,7 +34135,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" customFormat="1" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>1822</v>
+        <v>1826</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -34029,7 +34165,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
-        <v>1823</v>
+        <v>1827</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -34096,7 +34232,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
-        <v>1824</v>
+        <v>1828</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -34166,7 +34302,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="40" t="s">
-        <v>1825</v>
+        <v>1829</v>
       </c>
       <c r="B53" s="40"/>
       <c r="C53" s="40"/>
@@ -34220,7 +34356,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="14" t="s">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>946</v>
@@ -34258,7 +34394,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="40" t="s">
-        <v>1827</v>
+        <v>1831</v>
       </c>
       <c r="B57" s="40"/>
       <c r="C57" s="40"/>
@@ -34350,7 +34486,7 @@
     </row>
     <row r="61" s="7" customFormat="1" spans="1:3">
       <c r="A61" s="9" t="s">
-        <v>1828</v>
+        <v>1832</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -34380,7 +34516,7 @@
     <row r="64" s="7" customFormat="1"/>
     <row r="65" s="7" customFormat="1" spans="1:3">
       <c r="A65" s="9" t="s">
-        <v>1829</v>
+        <v>1833</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -34410,7 +34546,7 @@
     <row r="68" s="7" customFormat="1"/>
     <row r="69" s="7" customFormat="1" spans="1:3">
       <c r="A69" s="9" t="s">
-        <v>1830</v>
+        <v>1834</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -34440,7 +34576,7 @@
     <row r="72" s="7" customFormat="1"/>
     <row r="73" s="7" customFormat="1" spans="1:3">
       <c r="A73" s="9" t="s">
-        <v>1831</v>
+        <v>1835</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -34470,7 +34606,7 @@
     <row r="76" s="7" customFormat="1"/>
     <row r="77" s="7" customFormat="1" spans="1:3">
       <c r="A77" s="9" t="s">
-        <v>1832</v>
+        <v>1836</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -34500,7 +34636,7 @@
     <row r="80" s="7" customFormat="1"/>
     <row r="81" s="7" customFormat="1" spans="1:3">
       <c r="A81" s="9" t="s">
-        <v>1833</v>
+        <v>1837</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -34530,7 +34666,7 @@
     <row r="84" s="7" customFormat="1"/>
     <row r="85" s="7" customFormat="1" spans="1:3">
       <c r="A85" s="9" t="s">
-        <v>1834</v>
+        <v>1838</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -34560,7 +34696,7 @@
     <row r="88" s="7" customFormat="1"/>
     <row r="89" s="7" customFormat="1" spans="1:3">
       <c r="A89" s="9" t="s">
-        <v>1835</v>
+        <v>1839</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -34590,7 +34726,7 @@
     <row r="92" s="7" customFormat="1"/>
     <row r="93" s="7" customFormat="1" spans="1:3">
       <c r="A93" s="9" t="s">
-        <v>1836</v>
+        <v>1840</v>
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -34620,7 +34756,7 @@
     <row r="96" s="7" customFormat="1"/>
     <row r="97" s="7" customFormat="1" spans="1:3">
       <c r="A97" s="9" t="s">
-        <v>1837</v>
+        <v>1841</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -34650,7 +34786,7 @@
     <row r="100" s="7" customFormat="1"/>
     <row r="101" s="7" customFormat="1" spans="1:3">
       <c r="A101" s="9" t="s">
-        <v>1838</v>
+        <v>1842</v>
       </c>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -34680,7 +34816,7 @@
     <row r="104" s="7" customFormat="1"/>
     <row r="105" s="7" customFormat="1" spans="1:3">
       <c r="A105" s="9" t="s">
-        <v>1839</v>
+        <v>1843</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -34710,7 +34846,7 @@
     <row r="108" s="7" customFormat="1"/>
     <row r="109" s="7" customFormat="1" spans="1:3">
       <c r="A109" s="9" t="s">
-        <v>1840</v>
+        <v>1844</v>
       </c>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -34740,7 +34876,7 @@
     <row r="112" s="7" customFormat="1"/>
     <row r="113" s="7" customFormat="1" spans="1:3">
       <c r="A113" s="9" t="s">
-        <v>1841</v>
+        <v>1845</v>
       </c>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -34770,7 +34906,7 @@
     <row r="116" s="7" customFormat="1"/>
     <row r="117" s="7" customFormat="1" spans="1:3">
       <c r="A117" s="9" t="s">
-        <v>1842</v>
+        <v>1846</v>
       </c>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -34800,7 +34936,7 @@
     <row r="120" s="7" customFormat="1"/>
     <row r="121" s="7" customFormat="1" spans="1:3">
       <c r="A121" s="9" t="s">
-        <v>1843</v>
+        <v>1847</v>
       </c>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -34830,7 +34966,7 @@
     <row r="124" s="7" customFormat="1"/>
     <row r="125" s="7" customFormat="1" spans="1:3">
       <c r="A125" s="9" t="s">
-        <v>1844</v>
+        <v>1848</v>
       </c>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
@@ -34860,7 +34996,7 @@
     <row r="128" s="7" customFormat="1"/>
     <row r="129" s="7" customFormat="1" spans="1:3">
       <c r="A129" s="9" t="s">
-        <v>1845</v>
+        <v>1849</v>
       </c>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -34890,7 +35026,7 @@
     <row r="132" s="7" customFormat="1"/>
     <row r="133" s="7" customFormat="1" spans="1:3">
       <c r="A133" s="9" t="s">
-        <v>1846</v>
+        <v>1850</v>
       </c>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -34920,7 +35056,7 @@
     <row r="136" s="7" customFormat="1"/>
     <row r="137" s="7" customFormat="1" spans="1:3">
       <c r="A137" s="9" t="s">
-        <v>1847</v>
+        <v>1851</v>
       </c>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -34950,7 +35086,7 @@
     <row r="140" s="7" customFormat="1"/>
     <row r="141" s="7" customFormat="1" spans="1:3">
       <c r="A141" s="9" t="s">
-        <v>1848</v>
+        <v>1852</v>
       </c>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -34980,7 +35116,7 @@
     <row r="144" s="7" customFormat="1"/>
     <row r="145" s="7" customFormat="1" spans="1:3">
       <c r="A145" s="9" t="s">
-        <v>1849</v>
+        <v>1853</v>
       </c>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
@@ -35010,7 +35146,7 @@
     <row r="148" s="7" customFormat="1"/>
     <row r="149" s="7" customFormat="1" spans="1:3">
       <c r="A149" s="9" t="s">
-        <v>1850</v>
+        <v>1854</v>
       </c>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -35040,7 +35176,7 @@
     <row r="152" s="7" customFormat="1"/>
     <row r="153" s="7" customFormat="1" spans="1:3">
       <c r="A153" s="9" t="s">
-        <v>1851</v>
+        <v>1855</v>
       </c>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -35070,7 +35206,7 @@
     <row r="156" s="7" customFormat="1"/>
     <row r="157" s="7" customFormat="1" spans="1:3">
       <c r="A157" s="9" t="s">
-        <v>1852</v>
+        <v>1856</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -35100,7 +35236,7 @@
     <row r="160" s="7" customFormat="1"/>
     <row r="161" s="7" customFormat="1" spans="1:3">
       <c r="A161" s="9" t="s">
-        <v>1853</v>
+        <v>1857</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
@@ -35130,7 +35266,7 @@
     <row r="164" s="7" customFormat="1"/>
     <row r="165" s="7" customFormat="1" spans="1:3">
       <c r="A165" s="9" t="s">
-        <v>1854</v>
+        <v>1858</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -35160,7 +35296,7 @@
     <row r="168" s="7" customFormat="1"/>
     <row r="169" s="7" customFormat="1" spans="1:3">
       <c r="A169" s="9" t="s">
-        <v>1855</v>
+        <v>1859</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -35190,7 +35326,7 @@
     <row r="172" s="7" customFormat="1"/>
     <row r="173" s="7" customFormat="1" spans="1:3">
       <c r="A173" s="9" t="s">
-        <v>1856</v>
+        <v>1860</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -35220,7 +35356,7 @@
     <row r="176" s="7" customFormat="1"/>
     <row r="177" s="7" customFormat="1" spans="1:3">
       <c r="A177" s="9" t="s">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
@@ -35250,7 +35386,7 @@
     <row r="180" s="7" customFormat="1"/>
     <row r="181" s="7" customFormat="1" spans="1:3">
       <c r="A181" s="9" t="s">
-        <v>1858</v>
+        <v>1862</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
@@ -35280,7 +35416,7 @@
     <row r="184" s="7" customFormat="1"/>
     <row r="185" s="7" customFormat="1" spans="1:3">
       <c r="A185" s="9" t="s">
-        <v>1859</v>
+        <v>1863</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
@@ -35310,7 +35446,7 @@
     <row r="188" s="7" customFormat="1"/>
     <row r="189" s="7" customFormat="1" spans="1:3">
       <c r="A189" s="9" t="s">
-        <v>1860</v>
+        <v>1864</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
@@ -35340,7 +35476,7 @@
     <row r="192" s="7" customFormat="1"/>
     <row r="193" s="7" customFormat="1" spans="1:3">
       <c r="A193" s="9" t="s">
-        <v>1861</v>
+        <v>1865</v>
       </c>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
@@ -35370,7 +35506,7 @@
     <row r="196" s="7" customFormat="1"/>
     <row r="197" s="7" customFormat="1" spans="1:3">
       <c r="A197" s="9" t="s">
-        <v>1862</v>
+        <v>1866</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -35400,7 +35536,7 @@
     <row r="200" s="7" customFormat="1"/>
     <row r="201" s="7" customFormat="1" spans="1:3">
       <c r="A201" s="9" t="s">
-        <v>1863</v>
+        <v>1867</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
@@ -35430,7 +35566,7 @@
     <row r="204" s="7" customFormat="1"/>
     <row r="205" s="7" customFormat="1" spans="1:3">
       <c r="A205" s="9" t="s">
-        <v>1864</v>
+        <v>1868</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="9"/>
@@ -35460,7 +35596,7 @@
     <row r="208" s="7" customFormat="1"/>
     <row r="209" s="7" customFormat="1" spans="1:3">
       <c r="A209" s="9" t="s">
-        <v>1865</v>
+        <v>1869</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="9"/>
@@ -35490,7 +35626,7 @@
     <row r="212" s="7" customFormat="1"/>
     <row r="213" s="7" customFormat="1" spans="1:3">
       <c r="A213" s="9" t="s">
-        <v>1866</v>
+        <v>1870</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
@@ -35520,7 +35656,7 @@
     <row r="216" s="7" customFormat="1"/>
     <row r="217" s="7" customFormat="1" spans="1:3">
       <c r="A217" s="9" t="s">
-        <v>1867</v>
+        <v>1871</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
@@ -35550,7 +35686,7 @@
     <row r="220" s="7" customFormat="1"/>
     <row r="221" s="7" customFormat="1" spans="1:3">
       <c r="A221" s="9" t="s">
-        <v>1868</v>
+        <v>1872</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="9"/>
@@ -35580,7 +35716,7 @@
     <row r="224" s="7" customFormat="1"/>
     <row r="225" s="7" customFormat="1" spans="1:3">
       <c r="A225" s="9" t="s">
-        <v>1869</v>
+        <v>1873</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="9"/>
@@ -35610,7 +35746,7 @@
     <row r="228" s="7" customFormat="1"/>
     <row r="229" s="7" customFormat="1" spans="1:3">
       <c r="A229" s="9" t="s">
-        <v>1870</v>
+        <v>1874</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="9"/>
@@ -35640,7 +35776,7 @@
     <row r="232" s="7" customFormat="1"/>
     <row r="233" s="7" customFormat="1" spans="1:3">
       <c r="A233" s="9" t="s">
-        <v>1871</v>
+        <v>1875</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="9"/>
@@ -35670,7 +35806,7 @@
     <row r="236" s="7" customFormat="1"/>
     <row r="237" s="7" customFormat="1" spans="1:3">
       <c r="A237" s="9" t="s">
-        <v>1872</v>
+        <v>1876</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="9"/>
@@ -35700,7 +35836,7 @@
     <row r="240" s="7" customFormat="1"/>
     <row r="241" s="7" customFormat="1" spans="1:3">
       <c r="A241" s="9" t="s">
-        <v>1873</v>
+        <v>1877</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="9"/>
@@ -35730,7 +35866,7 @@
     <row r="244" s="7" customFormat="1"/>
     <row r="245" s="7" customFormat="1" spans="1:3">
       <c r="A245" s="9" t="s">
-        <v>1874</v>
+        <v>1878</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
@@ -35760,7 +35896,7 @@
     <row r="248" s="7" customFormat="1"/>
     <row r="249" s="7" customFormat="1" spans="1:3">
       <c r="A249" s="9" t="s">
-        <v>1875</v>
+        <v>1879</v>
       </c>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
@@ -35790,7 +35926,7 @@
     <row r="252" s="7" customFormat="1"/>
     <row r="253" s="7" customFormat="1" spans="1:3">
       <c r="A253" s="9" t="s">
-        <v>1876</v>
+        <v>1880</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
@@ -35820,7 +35956,7 @@
     <row r="256" s="7" customFormat="1"/>
     <row r="257" s="7" customFormat="1" spans="1:3">
       <c r="A257" s="9" t="s">
-        <v>1877</v>
+        <v>1881</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -35849,7 +35985,7 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="35" t="s">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="B261" s="35"/>
       <c r="C261" s="35"/>
@@ -35878,7 +36014,7 @@
     </row>
     <row r="265" spans="1:8">
       <c r="A265" s="36" t="s">
-        <v>1879</v>
+        <v>1883</v>
       </c>
       <c r="B265" s="36"/>
       <c r="C265" s="37"/>
@@ -35942,7 +36078,7 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="35" t="s">
-        <v>1880</v>
+        <v>1884</v>
       </c>
       <c r="B269" s="35"/>
       <c r="C269" s="35"/>
@@ -35971,7 +36107,7 @@
     </row>
     <row r="273" customFormat="1" spans="1:4">
       <c r="A273" s="48" t="s">
-        <v>1881</v>
+        <v>1885</v>
       </c>
       <c r="B273" s="48"/>
       <c r="C273" s="48"/>
@@ -36013,7 +36149,7 @@
     </row>
     <row r="277" customFormat="1" spans="1:4">
       <c r="A277" s="9" t="s">
-        <v>1882</v>
+        <v>1886</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
@@ -36051,7 +36187,7 @@
     </row>
     <row r="281" customFormat="1" spans="1:4">
       <c r="A281" s="9" t="s">
-        <v>1883</v>
+        <v>1887</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
@@ -36085,7 +36221,7 @@
     </row>
     <row r="285" customFormat="1" spans="1:4">
       <c r="A285" s="9" t="s">
-        <v>1884</v>
+        <v>1888</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
@@ -36113,7 +36249,7 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="9" t="s">
-        <v>1885</v>
+        <v>1889</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="9"/>
@@ -36142,7 +36278,7 @@
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="9" t="s">
-        <v>1882</v>
+        <v>1886</v>
       </c>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
@@ -36171,7 +36307,7 @@
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
-        <v>1886</v>
+        <v>1890</v>
       </c>
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
@@ -36200,7 +36336,7 @@
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
-        <v>1887</v>
+        <v>1891</v>
       </c>
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
@@ -36224,7 +36360,7 @@
         <v>1</v>
       </c>
       <c r="B303" s="14" t="s">
-        <v>1826</v>
+        <v>1830</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>6</v>
@@ -36235,7 +36371,7 @@
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
-        <v>1888</v>
+        <v>1892</v>
       </c>
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
@@ -36248,7 +36384,7 @@
         <v>855</v>
       </c>
       <c r="C306" s="10" t="s">
-        <v>1889</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -36264,7 +36400,7 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
-        <v>1890</v>
+        <v>1894</v>
       </c>
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
@@ -36277,7 +36413,7 @@
         <v>855</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>1889</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -36293,7 +36429,7 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
-        <v>1891</v>
+        <v>1895</v>
       </c>
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
@@ -36471,7 +36607,7 @@
   <sheetData>
     <row r="2" s="20" customFormat="1" spans="1:3">
       <c r="A2" s="21" t="s">
-        <v>1892</v>
+        <v>1896</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -36500,7 +36636,7 @@
     </row>
     <row r="6" s="20" customFormat="1" spans="1:3">
       <c r="A6" s="21" t="s">
-        <v>1893</v>
+        <v>1897</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -36529,7 +36665,7 @@
     </row>
     <row r="10" s="20" customFormat="1" spans="1:3">
       <c r="A10" s="21" t="s">
-        <v>1894</v>
+        <v>1898</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -36563,7 +36699,7 @@
     </row>
     <row r="14" s="20" customFormat="1" spans="1:3">
       <c r="A14" s="21" t="s">
-        <v>1895</v>
+        <v>1899</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -36597,7 +36733,7 @@
     </row>
     <row r="18" s="20" customFormat="1" spans="1:3">
       <c r="A18" s="21" t="s">
-        <v>1896</v>
+        <v>1900</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -36631,7 +36767,7 @@
     </row>
     <row r="22" s="20" customFormat="1" spans="1:3">
       <c r="A22" s="21" t="s">
-        <v>1897</v>
+        <v>1901</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -36665,7 +36801,7 @@
     </row>
     <row r="26" s="20" customFormat="1" spans="1:3">
       <c r="A26" s="21" t="s">
-        <v>1898</v>
+        <v>1902</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -36699,7 +36835,7 @@
     </row>
     <row r="30" s="20" customFormat="1" spans="1:4">
       <c r="A30" s="21" t="s">
-        <v>1899</v>
+        <v>1903</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -36716,7 +36852,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1900</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="32" s="20" customFormat="1" spans="1:4">
@@ -36730,7 +36866,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1901</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="33" s="20" customFormat="1" spans="1:3">
@@ -36740,7 +36876,7 @@
     </row>
     <row r="34" s="20" customFormat="1" spans="1:3">
       <c r="A34" s="21" t="s">
-        <v>1902</v>
+        <v>1906</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -36774,7 +36910,7 @@
     </row>
     <row r="38" s="20" customFormat="1" spans="1:3">
       <c r="A38" s="21" t="s">
-        <v>1903</v>
+        <v>1907</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -36808,7 +36944,7 @@
     </row>
     <row r="42" s="20" customFormat="1" spans="1:3">
       <c r="A42" s="21" t="s">
-        <v>1904</v>
+        <v>1908</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -36842,7 +36978,7 @@
     </row>
     <row r="46" s="20" customFormat="1" spans="1:3">
       <c r="A46" s="25" t="s">
-        <v>1905</v>
+        <v>1909</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
@@ -36871,7 +37007,7 @@
     </row>
     <row r="50" s="20" customFormat="1" spans="1:5">
       <c r="A50" s="21" t="s">
-        <v>1906</v>
+        <v>1910</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -36889,7 +37025,7 @@
         <v>539</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>1900</v>
+        <v>1904</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>4</v>
@@ -36906,7 +37042,7 @@
         <v>961</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>1901</v>
+        <v>1905</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>6</v>
@@ -36914,7 +37050,7 @@
     </row>
     <row r="54" s="20" customFormat="1" spans="1:5">
       <c r="A54" s="21" t="s">
-        <v>1907</v>
+        <v>1911</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -36935,7 +37071,7 @@
         <v>539</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>1900</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="56" s="20" customFormat="1" spans="1:5">
@@ -36952,7 +37088,7 @@
         <v>961</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>1908</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="57" s="20" customFormat="1" spans="1:5">
@@ -36964,7 +37100,7 @@
     </row>
     <row r="58" s="20" customFormat="1" spans="1:5">
       <c r="A58" s="25" t="s">
-        <v>1909</v>
+        <v>1913</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -36999,7 +37135,7 @@
     </row>
     <row r="62" s="20" customFormat="1" spans="1:5">
       <c r="A62" s="21" t="s">
-        <v>1910</v>
+        <v>1914</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -37017,10 +37153,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>1911</v>
+        <v>1915</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>1900</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="64" s="20" customFormat="1" spans="1:5">
@@ -37037,7 +37173,7 @@
         <v>961</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>1901</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="65" s="20" customFormat="1" spans="1:5">
@@ -37049,7 +37185,7 @@
     </row>
     <row r="66" s="20" customFormat="1" spans="1:5">
       <c r="A66" s="27" t="s">
-        <v>1912</v>
+        <v>1916</v>
       </c>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
@@ -37089,7 +37225,7 @@
     </row>
     <row r="70" s="20" customFormat="1" spans="1:5">
       <c r="A70" s="27" t="s">
-        <v>1913</v>
+        <v>1917</v>
       </c>
       <c r="B70" s="27"/>
       <c r="C70" s="27"/>
@@ -37124,7 +37260,7 @@
     </row>
     <row r="74" s="20" customFormat="1" spans="1:17">
       <c r="A74" s="21" t="s">
-        <v>1914</v>
+        <v>1918</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -37157,7 +37293,7 @@
         <v>1279</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>1915</v>
+        <v>1919</v>
       </c>
       <c r="F75" s="10" t="s">
         <v>844</v>
@@ -37190,10 +37326,10 @@
         <v>852</v>
       </c>
       <c r="P75" s="10" t="s">
-        <v>1916</v>
+        <v>1920</v>
       </c>
       <c r="Q75" s="10" t="s">
-        <v>1917</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="76" s="20" customFormat="1" spans="1:17">
@@ -37210,43 +37346,43 @@
         <v>961</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>1918</v>
+        <v>1922</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>1919</v>
+        <v>1923</v>
       </c>
       <c r="G76" s="11" t="s">
         <v>853</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>1920</v>
+        <v>1924</v>
       </c>
       <c r="I76" s="33">
         <v>6456788899</v>
       </c>
       <c r="J76" s="26" t="s">
-        <v>1921</v>
+        <v>1925</v>
       </c>
       <c r="K76" s="29" t="s">
-        <v>1922</v>
+        <v>1926</v>
       </c>
       <c r="L76" s="11" t="s">
-        <v>1923</v>
+        <v>1927</v>
       </c>
       <c r="M76" s="11" t="s">
-        <v>1924</v>
+        <v>1928</v>
       </c>
       <c r="N76" s="29" t="s">
         <v>1036</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>1925</v>
+        <v>1929</v>
       </c>
       <c r="P76" s="11" t="s">
-        <v>1926</v>
+        <v>1930</v>
       </c>
       <c r="Q76" s="11" t="s">
-        <v>1927</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="77" s="20" customFormat="1" spans="1:17">
@@ -37268,7 +37404,7 @@
     </row>
     <row r="78" s="20" customFormat="1" spans="1:17">
       <c r="A78" s="21" t="s">
-        <v>1928</v>
+        <v>1932</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
@@ -37354,7 +37490,7 @@
     </row>
     <row r="82" s="20" customFormat="1" spans="1:17">
       <c r="A82" s="27" t="s">
-        <v>1929</v>
+        <v>1933</v>
       </c>
       <c r="B82" s="27"/>
       <c r="C82" s="27"/>
@@ -37433,7 +37569,7 @@
     </row>
     <row r="86" s="20" customFormat="1" spans="1:17">
       <c r="A86" s="27" t="s">
-        <v>1930</v>
+        <v>1934</v>
       </c>
       <c r="B86" s="27"/>
       <c r="C86" s="27"/>
@@ -37512,7 +37648,7 @@
     </row>
     <row r="90" s="20" customFormat="1" spans="1:17">
       <c r="A90" s="27" t="s">
-        <v>1931</v>
+        <v>1935</v>
       </c>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
@@ -37577,7 +37713,7 @@
     </row>
     <row r="94" s="20" customFormat="1" spans="1:3">
       <c r="A94" s="21" t="s">
-        <v>1932</v>
+        <v>1936</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
@@ -37611,7 +37747,7 @@
     </row>
     <row r="98" s="20" customFormat="1" spans="1:3">
       <c r="A98" s="27" t="s">
-        <v>1933</v>
+        <v>1937</v>
       </c>
       <c r="B98" s="27"/>
       <c r="C98" s="27"/>
@@ -37640,7 +37776,7 @@
     </row>
     <row r="102" s="20" customFormat="1" spans="1:3">
       <c r="A102" s="27" t="s">
-        <v>1934</v>
+        <v>1938</v>
       </c>
       <c r="B102" s="27"/>
       <c r="C102" s="27"/>
@@ -37672,7 +37808,7 @@
     </row>
     <row r="106" s="20" customFormat="1" spans="1:3">
       <c r="A106" s="27" t="s">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
@@ -37704,7 +37840,7 @@
     </row>
     <row r="110" s="20" customFormat="1" spans="1:3">
       <c r="A110" s="27" t="s">
-        <v>1936</v>
+        <v>1940</v>
       </c>
       <c r="B110" s="27"/>
       <c r="C110" s="27"/>
@@ -37736,7 +37872,7 @@
     </row>
     <row r="114" s="20" customFormat="1" spans="1:3">
       <c r="A114" s="27" t="s">
-        <v>1937</v>
+        <v>1941</v>
       </c>
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
@@ -37770,7 +37906,7 @@
     </row>
     <row r="118" s="20" customFormat="1" spans="1:3">
       <c r="A118" s="21" t="s">
-        <v>1938</v>
+        <v>1942</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="21"/>
@@ -37799,7 +37935,7 @@
     </row>
     <row r="122" s="20" customFormat="1" spans="1:3">
       <c r="A122" s="21" t="s">
-        <v>1939</v>
+        <v>1943</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="21"/>
@@ -37828,7 +37964,7 @@
     </row>
     <row r="126" s="20" customFormat="1" spans="1:3">
       <c r="A126" s="21" t="s">
-        <v>1940</v>
+        <v>1944</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
@@ -37857,7 +37993,7 @@
     </row>
     <row r="130" s="20" customFormat="1" spans="1:3">
       <c r="A130" s="27" t="s">
-        <v>1941</v>
+        <v>1945</v>
       </c>
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
@@ -37889,7 +38025,7 @@
     </row>
     <row r="134" s="20" customFormat="1" spans="1:3">
       <c r="A134" s="27" t="s">
-        <v>1942</v>
+        <v>1946</v>
       </c>
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
@@ -37921,7 +38057,7 @@
     </row>
     <row r="138" s="20" customFormat="1" spans="1:3">
       <c r="A138" s="27" t="s">
-        <v>1943</v>
+        <v>1947</v>
       </c>
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
@@ -37950,7 +38086,7 @@
     </row>
     <row r="142" s="20" customFormat="1" spans="1:3">
       <c r="A142" s="27" t="s">
-        <v>1944</v>
+        <v>1948</v>
       </c>
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
@@ -37979,7 +38115,7 @@
     </row>
     <row r="146" s="20" customFormat="1" spans="1:3">
       <c r="A146" s="27" t="s">
-        <v>1945</v>
+        <v>1949</v>
       </c>
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
@@ -38008,7 +38144,7 @@
     </row>
     <row r="150" s="20" customFormat="1" spans="1:3">
       <c r="A150" s="27" t="s">
-        <v>1946</v>
+        <v>1950</v>
       </c>
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
@@ -38037,7 +38173,7 @@
     </row>
     <row r="154" s="20" customFormat="1" spans="1:3">
       <c r="A154" s="27" t="s">
-        <v>1947</v>
+        <v>1951</v>
       </c>
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
@@ -38066,7 +38202,7 @@
     </row>
     <row r="158" s="20" customFormat="1" spans="1:3">
       <c r="A158" s="27" t="s">
-        <v>1948</v>
+        <v>1952</v>
       </c>
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
@@ -38095,7 +38231,7 @@
     </row>
     <row r="162" s="20" customFormat="1" spans="1:3">
       <c r="A162" s="27" t="s">
-        <v>1949</v>
+        <v>1953</v>
       </c>
       <c r="B162" s="27"/>
       <c r="C162" s="27"/>
@@ -38124,7 +38260,7 @@
     </row>
     <row r="166" s="20" customFormat="1" spans="1:3">
       <c r="A166" s="27" t="s">
-        <v>1950</v>
+        <v>1954</v>
       </c>
       <c r="B166" s="27"/>
       <c r="C166" s="27"/>
@@ -38153,7 +38289,7 @@
     </row>
     <row r="170" s="20" customFormat="1" spans="1:3">
       <c r="A170" s="27" t="s">
-        <v>1951</v>
+        <v>1955</v>
       </c>
       <c r="B170" s="27"/>
       <c r="C170" s="27"/>
@@ -38182,7 +38318,7 @@
     </row>
     <row r="174" s="20" customFormat="1" spans="1:3">
       <c r="A174" s="27" t="s">
-        <v>1952</v>
+        <v>1956</v>
       </c>
       <c r="B174" s="27"/>
       <c r="C174" s="27"/>
@@ -38211,7 +38347,7 @@
     </row>
     <row r="178" s="20" customFormat="1" spans="1:3">
       <c r="A178" s="27" t="s">
-        <v>1953</v>
+        <v>1957</v>
       </c>
       <c r="B178" s="27"/>
       <c r="C178" s="27"/>
@@ -38240,7 +38376,7 @@
     </row>
     <row r="182" s="20" customFormat="1" spans="1:4">
       <c r="A182" s="21" t="s">
-        <v>1954</v>
+        <v>1958</v>
       </c>
       <c r="B182" s="21"/>
       <c r="C182" s="21"/>
@@ -38276,7 +38412,7 @@
     </row>
     <row r="186" s="20" customFormat="1" spans="1:3">
       <c r="A186" s="27" t="s">
-        <v>1955</v>
+        <v>1959</v>
       </c>
       <c r="B186" s="27"/>
       <c r="C186" s="27"/>
@@ -38305,7 +38441,7 @@
     </row>
     <row r="190" s="20" customFormat="1" spans="1:4">
       <c r="A190" s="27" t="s">
-        <v>1956</v>
+        <v>1960</v>
       </c>
       <c r="B190" s="27"/>
       <c r="C190" s="27"/>
@@ -38341,7 +38477,7 @@
     </row>
     <row r="194" s="20" customFormat="1" spans="1:3">
       <c r="A194" s="27" t="s">
-        <v>1957</v>
+        <v>1961</v>
       </c>
       <c r="B194" s="27"/>
       <c r="C194" s="27"/>
@@ -38370,7 +38506,7 @@
     </row>
     <row r="198" s="20" customFormat="1" spans="1:3">
       <c r="A198" s="27" t="s">
-        <v>1958</v>
+        <v>1962</v>
       </c>
       <c r="B198" s="27"/>
       <c r="C198" s="27"/>
@@ -38399,7 +38535,7 @@
     </row>
     <row r="202" s="20" customFormat="1" spans="1:3">
       <c r="A202" s="27" t="s">
-        <v>1959</v>
+        <v>1963</v>
       </c>
       <c r="B202" s="27"/>
       <c r="C202" s="27"/>
@@ -38863,7 +38999,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1960</v>
+        <v>1964</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -38891,7 +39027,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>1961</v>
+        <v>1965</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -38919,7 +39055,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>1962</v>
+        <v>1966</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -38947,7 +39083,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>1963</v>
+        <v>1967</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -38975,7 +39111,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>1964</v>
+        <v>1968</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -39003,7 +39139,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>1965</v>
+        <v>1969</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -39031,7 +39167,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>1966</v>
+        <v>1970</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -39059,7 +39195,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>1967</v>
+        <v>1971</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -39087,7 +39223,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>1968</v>
+        <v>1972</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -39115,7 +39251,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>1969</v>
+        <v>1973</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -39143,7 +39279,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>1970</v>
+        <v>1974</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -39164,7 +39300,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1971</v>
+        <v>1975</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>6</v>
@@ -39173,7 +39309,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>1972</v>
+        <v>1976</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -39246,7 +39382,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1973</v>
+        <v>1977</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -39274,7 +39410,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>1974</v>
+        <v>1978</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -39302,7 +39438,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>1975</v>
+        <v>1979</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -39330,7 +39466,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>1976</v>
+        <v>1980</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -39358,7 +39494,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>1977</v>
+        <v>1981</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -39386,7 +39522,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>1978</v>
+        <v>1982</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -39396,34 +39532,34 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1983</v>
+        <v>1987</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>542</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>4</v>
@@ -39440,28 +39576,28 @@
         <v>1282</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1989</v>
+        <v>1993</v>
       </c>
       <c r="H23" s="147" t="s">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="J23" s="147" t="s">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="K23" t="s">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>6</v>
@@ -39480,7 +39616,7 @@
     </row>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -39508,7 +39644,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>1995</v>
+        <v>1999</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -39536,7 +39672,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -39546,40 +39682,40 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1983</v>
+        <v>1987</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>1997</v>
+        <v>2001</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>4</v>
@@ -39596,34 +39732,34 @@
         <v>1282</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H35" s="147" t="s">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="K35" s="147" t="s">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="L35" t="s">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>6</v>
@@ -39632,7 +39768,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -43566,7 +43702,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -43594,7 +43730,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2003</v>
+        <v>2007</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -43622,7 +43758,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -43650,7 +43786,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -43678,7 +43814,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -43706,7 +43842,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -43734,7 +43870,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -43762,7 +43898,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -43790,7 +43926,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -43818,7 +43954,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -43846,7 +43982,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -43867,7 +44003,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1971</v>
+        <v>1975</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>6</v>
@@ -43876,7 +44012,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -43946,7 +44082,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -43974,7 +44110,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44002,7 +44138,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44030,7 +44166,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44058,7 +44194,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -44086,7 +44222,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -44096,34 +44232,34 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1983</v>
+        <v>1987</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>542</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>4</v>
@@ -44140,28 +44276,28 @@
         <v>1282</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H23" s="147" t="s">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="J23" s="147" t="s">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>6</v>
@@ -44180,7 +44316,7 @@
     </row>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -44208,7 +44344,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -44236,7 +44372,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2022</v>
+        <v>2026</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -44246,40 +44382,40 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1983</v>
+        <v>1987</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>1997</v>
+        <v>2001</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>4</v>
@@ -44296,34 +44432,34 @@
         <v>1282</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H35" s="147" t="s">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="K35" s="147" t="s">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>6</v>
@@ -44332,7 +44468,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2023</v>
+        <v>2027</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -44393,7 +44529,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2024</v>
+        <v>2028</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -44421,7 +44557,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2025</v>
+        <v>2029</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44449,7 +44585,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2026</v>
+        <v>2030</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44477,7 +44613,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2027</v>
+        <v>2031</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44505,7 +44641,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2028</v>
+        <v>2032</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -44533,7 +44669,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2029</v>
+        <v>2033</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -44561,7 +44697,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2030</v>
+        <v>2034</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -44589,7 +44725,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2031</v>
+        <v>2035</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -44617,7 +44753,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2032</v>
+        <v>2036</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -44645,7 +44781,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2033</v>
+        <v>2037</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -44673,7 +44809,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2034</v>
+        <v>2038</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -44735,7 +44871,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2035</v>
+        <v>2039</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -44763,7 +44899,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2036</v>
+        <v>2040</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44791,7 +44927,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2037</v>
+        <v>2041</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44819,7 +44955,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2038</v>
+        <v>2042</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44847,7 +44983,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2039</v>
+        <v>2043</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -44875,7 +45011,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2040</v>
+        <v>2044</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -44903,7 +45039,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2041</v>
+        <v>2045</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -44931,7 +45067,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2042</v>
+        <v>2046</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -44959,7 +45095,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2043</v>
+        <v>2047</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -44987,7 +45123,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2044</v>
+        <v>2048</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -45015,7 +45151,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2045</v>
+        <v>2049</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -45077,7 +45213,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2046</v>
+        <v>2050</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45105,7 +45241,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2047</v>
+        <v>2051</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -45133,7 +45269,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2048</v>
+        <v>2052</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -45161,7 +45297,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2049</v>
+        <v>2053</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -45189,7 +45325,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2050</v>
+        <v>2054</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -45217,7 +45353,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2051</v>
+        <v>2055</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -45245,7 +45381,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2052</v>
+        <v>2056</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -45273,7 +45409,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2053</v>
+        <v>2057</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -45301,7 +45437,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2054</v>
+        <v>2058</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -45329,7 +45465,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2055</v>
+        <v>2059</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -45357,7 +45493,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2056</v>
+        <v>2060</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -45385,7 +45521,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2057</v>
+        <v>2061</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -45413,7 +45549,7 @@
     <row r="48" customFormat="1"/>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>2058</v>
+        <v>2062</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -45441,7 +45577,7 @@
     <row r="52" customFormat="1"/>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>2059</v>
+        <v>2063</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -45469,7 +45605,7 @@
     <row r="56" customFormat="1"/>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>2060</v>
+        <v>2064</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -45497,7 +45633,7 @@
     <row r="60" customFormat="1"/>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>2061</v>
+        <v>2065</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -45525,7 +45661,7 @@
     <row r="64" customFormat="1"/>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>2062</v>
+        <v>2066</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -45553,7 +45689,7 @@
     <row r="68" customFormat="1"/>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>2063</v>
+        <v>2067</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -45581,7 +45717,7 @@
     <row r="72" customFormat="1"/>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>2064</v>
+        <v>2068</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -45609,7 +45745,7 @@
     <row r="76" customFormat="1"/>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>2065</v>
+        <v>2069</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -45637,7 +45773,7 @@
     <row r="80" customFormat="1"/>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>2066</v>
+        <v>2070</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -45665,7 +45801,7 @@
     <row r="84" customFormat="1"/>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>2067</v>
+        <v>2071</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -45692,7 +45828,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>2068</v>
+        <v>2072</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -45766,7 +45902,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2069</v>
+        <v>2073</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45794,7 +45930,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2070</v>
+        <v>2074</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -45822,7 +45958,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2071</v>
+        <v>2075</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -45850,7 +45986,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2072</v>
+        <v>2076</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -45878,7 +46014,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2073</v>
+        <v>2077</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -45906,7 +46042,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2074</v>
+        <v>2078</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -45934,7 +46070,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2075</v>
+        <v>2079</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -45962,7 +46098,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2076</v>
+        <v>2080</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -45990,7 +46126,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2077</v>
+        <v>2081</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -46018,7 +46154,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2078</v>
+        <v>2082</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -46046,7 +46182,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2079</v>
+        <v>2083</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -46074,7 +46210,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2080</v>
+        <v>2084</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -46102,7 +46238,7 @@
     <row r="48" customFormat="1"/>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>2081</v>
+        <v>2085</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -46130,7 +46266,7 @@
     <row r="52" customFormat="1"/>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>2082</v>
+        <v>2086</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -46158,7 +46294,7 @@
     <row r="56" customFormat="1"/>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>2083</v>
+        <v>2087</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -46186,7 +46322,7 @@
     <row r="60" customFormat="1"/>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>2084</v>
+        <v>2088</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -46214,7 +46350,7 @@
     <row r="64" customFormat="1"/>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>2085</v>
+        <v>2089</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -46242,7 +46378,7 @@
     <row r="68" customFormat="1"/>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>2086</v>
+        <v>2090</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -46270,7 +46406,7 @@
     <row r="72" customFormat="1"/>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>2087</v>
+        <v>2091</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -46298,7 +46434,7 @@
     <row r="76" customFormat="1"/>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>2088</v>
+        <v>2092</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -46326,7 +46462,7 @@
     <row r="80" customFormat="1"/>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>2089</v>
+        <v>2093</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -46354,7 +46490,7 @@
     <row r="84" customFormat="1"/>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>2090</v>
+        <v>2094</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -46382,7 +46518,7 @@
     <row r="88" customFormat="1"/>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>2091</v>
+        <v>2095</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>

</xml_diff>

<commit_message>
Implemented Wifi Stability Xp8
</commit_message>
<xml_diff>
--- a/src/test/resources/documents/XP5S_All_TC.xlsx
+++ b/src/test/resources/documents/XP5S_All_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" tabRatio="656" firstSheet="12" activeTab="12"/>
+    <workbookView windowWidth="19890" windowHeight="7935" tabRatio="656" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,12 @@
     <sheet name="XP5S_SonimCare" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <oleSize ref="A443:F493"/>
+  <oleSize ref="A289:F339"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097">
   <si>
     <t>Sonimcare</t>
   </si>
@@ -5424,6 +5424,9 @@
   </si>
   <si>
     <t>XP8_TC_004_Stability_Enable_Disable_BT_And_Scan_BT_Devices</t>
+  </si>
+  <si>
+    <t>XP8_TC_001_Stability_Connection_and_Disconnection_Secured_Wifi_DeviceSettings</t>
   </si>
   <si>
     <t>XP8_TC_01_Stability_Setting_Up_Preconditions_Email</t>
@@ -6346,10 +6349,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -6429,21 +6432,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6457,9 +6461,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6479,71 +6544,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6624,25 +6627,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6660,61 +6657,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6732,7 +6699,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6750,55 +6801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6908,11 +6911,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6959,23 +6979,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6994,162 +7008,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -28122,10 +28125,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AY491"/>
+  <dimension ref="A1:AY499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
-      <selection activeCell="F478" sqref="F478"/>
+    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
+      <selection activeCell="G500" sqref="G500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -33139,8 +33142,71 @@
         <v>6</v>
       </c>
     </row>
+    <row r="493" s="7" customFormat="1" spans="1:3">
+      <c r="A493" s="9" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B493" s="9"/>
+      <c r="C493" s="9"/>
+    </row>
+    <row r="494" s="7" customFormat="1" spans="1:3">
+      <c r="A494" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B494" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="C494" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="495" s="7" customFormat="1" spans="1:3">
+      <c r="A495" s="11">
+        <v>1</v>
+      </c>
+      <c r="B495" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C495" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="496" s="7" customFormat="1" spans="1:3">
+      <c r="A496"/>
+      <c r="B496"/>
+      <c r="C496"/>
+    </row>
+    <row r="497" s="7" customFormat="1" spans="1:3">
+      <c r="A497" s="9" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B497" s="9"/>
+      <c r="C497" s="9"/>
+    </row>
+    <row r="498" s="7" customFormat="1" spans="1:3">
+      <c r="A498" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B498" s="10" t="s">
+        <v>855</v>
+      </c>
+      <c r="C498" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="499" s="7" customFormat="1" spans="1:3">
+      <c r="A499" s="11">
+        <v>1</v>
+      </c>
+      <c r="B499" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C499" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="123">
+  <mergeCells count="125">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A9:C9"/>
@@ -33264,6 +33330,8 @@
     <mergeCell ref="A481:C481"/>
     <mergeCell ref="A485:C485"/>
     <mergeCell ref="A489:C489"/>
+    <mergeCell ref="A493:C493"/>
+    <mergeCell ref="A497:C497"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B47" r:id="rId1" display="www.google.co.in"/>
@@ -33464,7 +33532,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="9" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -33485,16 +33553,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="9" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -33516,7 +33584,7 @@
         <v>1477</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="23" customFormat="1" ht="75" spans="1:6">
@@ -33527,22 +33595,22 @@
         <v>1479</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="9" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -33564,7 +33632,7 @@
         <v>1477</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>1210</v>
@@ -33578,25 +33646,25 @@
         <v>1479</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="9" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -33626,19 +33694,19 @@
         <v>1479</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>1221</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="9" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -33660,13 +33728,13 @@
         <v>570</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>529</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -33674,31 +33742,31 @@
         <v>1</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>573</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="E35" s="45" t="s">
         <v>1071</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>530</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="9" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -33764,8 +33832,8 @@
   <sheetPr/>
   <dimension ref="A1:L315"/>
   <sheetViews>
-    <sheetView topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="G289" sqref="G289"/>
+    <sheetView topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A293" sqref="A293:C293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -33785,7 +33853,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="35" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -33815,7 +33883,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="35" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -33845,7 +33913,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="35" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -33875,7 +33943,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:8">
       <c r="A13" s="36" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>
@@ -33940,7 +34008,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="35" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -33970,7 +34038,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="35" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -34000,7 +34068,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:4">
       <c r="A25" s="39" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -34042,7 +34110,7 @@
     </row>
     <row r="29" customFormat="1" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -34075,7 +34143,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -34105,7 +34173,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -34135,7 +34203,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" customFormat="1" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -34165,7 +34233,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -34232,7 +34300,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -34302,7 +34370,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="40" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="B53" s="40"/>
       <c r="C53" s="40"/>
@@ -34356,7 +34424,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="14" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>946</v>
@@ -34394,7 +34462,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="40" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
       <c r="B57" s="40"/>
       <c r="C57" s="40"/>
@@ -34486,7 +34554,7 @@
     </row>
     <row r="61" s="7" customFormat="1" spans="1:3">
       <c r="A61" s="9" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -34516,7 +34584,7 @@
     <row r="64" s="7" customFormat="1"/>
     <row r="65" s="7" customFormat="1" spans="1:3">
       <c r="A65" s="9" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -34546,7 +34614,7 @@
     <row r="68" s="7" customFormat="1"/>
     <row r="69" s="7" customFormat="1" spans="1:3">
       <c r="A69" s="9" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -34576,7 +34644,7 @@
     <row r="72" s="7" customFormat="1"/>
     <row r="73" s="7" customFormat="1" spans="1:3">
       <c r="A73" s="9" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -34606,7 +34674,7 @@
     <row r="76" s="7" customFormat="1"/>
     <row r="77" s="7" customFormat="1" spans="1:3">
       <c r="A77" s="9" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -34636,7 +34704,7 @@
     <row r="80" s="7" customFormat="1"/>
     <row r="81" s="7" customFormat="1" spans="1:3">
       <c r="A81" s="9" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -34666,7 +34734,7 @@
     <row r="84" s="7" customFormat="1"/>
     <row r="85" s="7" customFormat="1" spans="1:3">
       <c r="A85" s="9" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -34696,7 +34764,7 @@
     <row r="88" s="7" customFormat="1"/>
     <row r="89" s="7" customFormat="1" spans="1:3">
       <c r="A89" s="9" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -34726,7 +34794,7 @@
     <row r="92" s="7" customFormat="1"/>
     <row r="93" s="7" customFormat="1" spans="1:3">
       <c r="A93" s="9" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -34756,7 +34824,7 @@
     <row r="96" s="7" customFormat="1"/>
     <row r="97" s="7" customFormat="1" spans="1:3">
       <c r="A97" s="9" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -34786,7 +34854,7 @@
     <row r="100" s="7" customFormat="1"/>
     <row r="101" s="7" customFormat="1" spans="1:3">
       <c r="A101" s="9" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -34816,7 +34884,7 @@
     <row r="104" s="7" customFormat="1"/>
     <row r="105" s="7" customFormat="1" spans="1:3">
       <c r="A105" s="9" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -34846,7 +34914,7 @@
     <row r="108" s="7" customFormat="1"/>
     <row r="109" s="7" customFormat="1" spans="1:3">
       <c r="A109" s="9" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -34876,7 +34944,7 @@
     <row r="112" s="7" customFormat="1"/>
     <row r="113" s="7" customFormat="1" spans="1:3">
       <c r="A113" s="9" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -34906,7 +34974,7 @@
     <row r="116" s="7" customFormat="1"/>
     <row r="117" s="7" customFormat="1" spans="1:3">
       <c r="A117" s="9" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -34936,7 +35004,7 @@
     <row r="120" s="7" customFormat="1"/>
     <row r="121" s="7" customFormat="1" spans="1:3">
       <c r="A121" s="9" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -34966,7 +35034,7 @@
     <row r="124" s="7" customFormat="1"/>
     <row r="125" s="7" customFormat="1" spans="1:3">
       <c r="A125" s="9" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
@@ -34996,7 +35064,7 @@
     <row r="128" s="7" customFormat="1"/>
     <row r="129" s="7" customFormat="1" spans="1:3">
       <c r="A129" s="9" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -35026,7 +35094,7 @@
     <row r="132" s="7" customFormat="1"/>
     <row r="133" s="7" customFormat="1" spans="1:3">
       <c r="A133" s="9" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -35056,7 +35124,7 @@
     <row r="136" s="7" customFormat="1"/>
     <row r="137" s="7" customFormat="1" spans="1:3">
       <c r="A137" s="9" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -35086,7 +35154,7 @@
     <row r="140" s="7" customFormat="1"/>
     <row r="141" s="7" customFormat="1" spans="1:3">
       <c r="A141" s="9" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -35116,7 +35184,7 @@
     <row r="144" s="7" customFormat="1"/>
     <row r="145" s="7" customFormat="1" spans="1:3">
       <c r="A145" s="9" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
@@ -35146,7 +35214,7 @@
     <row r="148" s="7" customFormat="1"/>
     <row r="149" s="7" customFormat="1" spans="1:3">
       <c r="A149" s="9" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -35176,7 +35244,7 @@
     <row r="152" s="7" customFormat="1"/>
     <row r="153" s="7" customFormat="1" spans="1:3">
       <c r="A153" s="9" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -35206,7 +35274,7 @@
     <row r="156" s="7" customFormat="1"/>
     <row r="157" s="7" customFormat="1" spans="1:3">
       <c r="A157" s="9" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -35236,7 +35304,7 @@
     <row r="160" s="7" customFormat="1"/>
     <row r="161" s="7" customFormat="1" spans="1:3">
       <c r="A161" s="9" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
@@ -35266,7 +35334,7 @@
     <row r="164" s="7" customFormat="1"/>
     <row r="165" s="7" customFormat="1" spans="1:3">
       <c r="A165" s="9" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -35296,7 +35364,7 @@
     <row r="168" s="7" customFormat="1"/>
     <row r="169" s="7" customFormat="1" spans="1:3">
       <c r="A169" s="9" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -35326,7 +35394,7 @@
     <row r="172" s="7" customFormat="1"/>
     <row r="173" s="7" customFormat="1" spans="1:3">
       <c r="A173" s="9" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -35356,7 +35424,7 @@
     <row r="176" s="7" customFormat="1"/>
     <row r="177" s="7" customFormat="1" spans="1:3">
       <c r="A177" s="9" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
@@ -35386,7 +35454,7 @@
     <row r="180" s="7" customFormat="1"/>
     <row r="181" s="7" customFormat="1" spans="1:3">
       <c r="A181" s="9" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
@@ -35416,7 +35484,7 @@
     <row r="184" s="7" customFormat="1"/>
     <row r="185" s="7" customFormat="1" spans="1:3">
       <c r="A185" s="9" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
@@ -35446,7 +35514,7 @@
     <row r="188" s="7" customFormat="1"/>
     <row r="189" s="7" customFormat="1" spans="1:3">
       <c r="A189" s="9" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
@@ -35476,7 +35544,7 @@
     <row r="192" s="7" customFormat="1"/>
     <row r="193" s="7" customFormat="1" spans="1:3">
       <c r="A193" s="9" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
@@ -35506,7 +35574,7 @@
     <row r="196" s="7" customFormat="1"/>
     <row r="197" s="7" customFormat="1" spans="1:3">
       <c r="A197" s="9" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -35536,7 +35604,7 @@
     <row r="200" s="7" customFormat="1"/>
     <row r="201" s="7" customFormat="1" spans="1:3">
       <c r="A201" s="9" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
@@ -35566,7 +35634,7 @@
     <row r="204" s="7" customFormat="1"/>
     <row r="205" s="7" customFormat="1" spans="1:3">
       <c r="A205" s="9" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="B205" s="9"/>
       <c r="C205" s="9"/>
@@ -35596,7 +35664,7 @@
     <row r="208" s="7" customFormat="1"/>
     <row r="209" s="7" customFormat="1" spans="1:3">
       <c r="A209" s="9" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="B209" s="9"/>
       <c r="C209" s="9"/>
@@ -35626,7 +35694,7 @@
     <row r="212" s="7" customFormat="1"/>
     <row r="213" s="7" customFormat="1" spans="1:3">
       <c r="A213" s="9" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
@@ -35656,7 +35724,7 @@
     <row r="216" s="7" customFormat="1"/>
     <row r="217" s="7" customFormat="1" spans="1:3">
       <c r="A217" s="9" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
@@ -35686,7 +35754,7 @@
     <row r="220" s="7" customFormat="1"/>
     <row r="221" s="7" customFormat="1" spans="1:3">
       <c r="A221" s="9" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="B221" s="9"/>
       <c r="C221" s="9"/>
@@ -35716,7 +35784,7 @@
     <row r="224" s="7" customFormat="1"/>
     <row r="225" s="7" customFormat="1" spans="1:3">
       <c r="A225" s="9" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
       <c r="B225" s="9"/>
       <c r="C225" s="9"/>
@@ -35746,7 +35814,7 @@
     <row r="228" s="7" customFormat="1"/>
     <row r="229" s="7" customFormat="1" spans="1:3">
       <c r="A229" s="9" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="B229" s="9"/>
       <c r="C229" s="9"/>
@@ -35776,7 +35844,7 @@
     <row r="232" s="7" customFormat="1"/>
     <row r="233" s="7" customFormat="1" spans="1:3">
       <c r="A233" s="9" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="B233" s="9"/>
       <c r="C233" s="9"/>
@@ -35806,7 +35874,7 @@
     <row r="236" s="7" customFormat="1"/>
     <row r="237" s="7" customFormat="1" spans="1:3">
       <c r="A237" s="9" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="B237" s="9"/>
       <c r="C237" s="9"/>
@@ -35836,7 +35904,7 @@
     <row r="240" s="7" customFormat="1"/>
     <row r="241" s="7" customFormat="1" spans="1:3">
       <c r="A241" s="9" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="B241" s="9"/>
       <c r="C241" s="9"/>
@@ -35866,7 +35934,7 @@
     <row r="244" s="7" customFormat="1"/>
     <row r="245" s="7" customFormat="1" spans="1:3">
       <c r="A245" s="9" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
@@ -35896,7 +35964,7 @@
     <row r="248" s="7" customFormat="1"/>
     <row r="249" s="7" customFormat="1" spans="1:3">
       <c r="A249" s="9" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
@@ -35926,7 +35994,7 @@
     <row r="252" s="7" customFormat="1"/>
     <row r="253" s="7" customFormat="1" spans="1:3">
       <c r="A253" s="9" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
@@ -35956,7 +36024,7 @@
     <row r="256" s="7" customFormat="1"/>
     <row r="257" s="7" customFormat="1" spans="1:3">
       <c r="A257" s="9" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
@@ -35985,7 +36053,7 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="35" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="B261" s="35"/>
       <c r="C261" s="35"/>
@@ -36014,7 +36082,7 @@
     </row>
     <row r="265" spans="1:8">
       <c r="A265" s="36" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="B265" s="36"/>
       <c r="C265" s="37"/>
@@ -36078,7 +36146,7 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="35" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="B269" s="35"/>
       <c r="C269" s="35"/>
@@ -36107,7 +36175,7 @@
     </row>
     <row r="273" customFormat="1" spans="1:4">
       <c r="A273" s="48" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="B273" s="48"/>
       <c r="C273" s="48"/>
@@ -36149,7 +36217,7 @@
     </row>
     <row r="277" customFormat="1" spans="1:4">
       <c r="A277" s="9" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
@@ -36187,7 +36255,7 @@
     </row>
     <row r="281" customFormat="1" spans="1:4">
       <c r="A281" s="9" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
@@ -36221,7 +36289,7 @@
     </row>
     <row r="285" customFormat="1" spans="1:4">
       <c r="A285" s="9" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
@@ -36249,7 +36317,7 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="9" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="B289" s="9"/>
       <c r="C289" s="9"/>
@@ -36278,7 +36346,7 @@
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="9" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
@@ -36307,7 +36375,7 @@
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
@@ -36336,7 +36404,7 @@
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
@@ -36360,7 +36428,7 @@
         <v>1</v>
       </c>
       <c r="B303" s="14" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>6</v>
@@ -36371,7 +36439,7 @@
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
@@ -36384,7 +36452,7 @@
         <v>855</v>
       </c>
       <c r="C306" s="10" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="307" spans="1:3">
@@ -36400,7 +36468,7 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="1" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
@@ -36413,7 +36481,7 @@
         <v>855</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -36429,7 +36497,7 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="1" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
@@ -36607,7 +36675,7 @@
   <sheetData>
     <row r="2" s="20" customFormat="1" spans="1:3">
       <c r="A2" s="21" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -36636,7 +36704,7 @@
     </row>
     <row r="6" s="20" customFormat="1" spans="1:3">
       <c r="A6" s="21" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -36665,7 +36733,7 @@
     </row>
     <row r="10" s="20" customFormat="1" spans="1:3">
       <c r="A10" s="21" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -36699,7 +36767,7 @@
     </row>
     <row r="14" s="20" customFormat="1" spans="1:3">
       <c r="A14" s="21" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -36733,7 +36801,7 @@
     </row>
     <row r="18" s="20" customFormat="1" spans="1:3">
       <c r="A18" s="21" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -36767,7 +36835,7 @@
     </row>
     <row r="22" s="20" customFormat="1" spans="1:3">
       <c r="A22" s="21" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -36801,7 +36869,7 @@
     </row>
     <row r="26" s="20" customFormat="1" spans="1:3">
       <c r="A26" s="21" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -36835,7 +36903,7 @@
     </row>
     <row r="30" s="20" customFormat="1" spans="1:4">
       <c r="A30" s="21" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -36852,7 +36920,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="32" s="20" customFormat="1" spans="1:4">
@@ -36866,7 +36934,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="33" s="20" customFormat="1" spans="1:3">
@@ -36876,7 +36944,7 @@
     </row>
     <row r="34" s="20" customFormat="1" spans="1:3">
       <c r="A34" s="21" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -36910,7 +36978,7 @@
     </row>
     <row r="38" s="20" customFormat="1" spans="1:3">
       <c r="A38" s="21" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -36944,7 +37012,7 @@
     </row>
     <row r="42" s="20" customFormat="1" spans="1:3">
       <c r="A42" s="21" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -36978,7 +37046,7 @@
     </row>
     <row r="46" s="20" customFormat="1" spans="1:3">
       <c r="A46" s="25" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
@@ -37007,7 +37075,7 @@
     </row>
     <row r="50" s="20" customFormat="1" spans="1:5">
       <c r="A50" s="21" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -37025,7 +37093,7 @@
         <v>539</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>4</v>
@@ -37042,7 +37110,7 @@
         <v>961</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>6</v>
@@ -37050,7 +37118,7 @@
     </row>
     <row r="54" s="20" customFormat="1" spans="1:5">
       <c r="A54" s="21" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -37071,7 +37139,7 @@
         <v>539</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="56" s="20" customFormat="1" spans="1:5">
@@ -37088,7 +37156,7 @@
         <v>961</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="57" s="20" customFormat="1" spans="1:5">
@@ -37100,7 +37168,7 @@
     </row>
     <row r="58" s="20" customFormat="1" spans="1:5">
       <c r="A58" s="25" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -37135,7 +37203,7 @@
     </row>
     <row r="62" s="20" customFormat="1" spans="1:5">
       <c r="A62" s="21" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -37153,10 +37221,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="64" s="20" customFormat="1" spans="1:5">
@@ -37173,7 +37241,7 @@
         <v>961</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="65" s="20" customFormat="1" spans="1:5">
@@ -37185,7 +37253,7 @@
     </row>
     <row r="66" s="20" customFormat="1" spans="1:5">
       <c r="A66" s="27" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
@@ -37225,7 +37293,7 @@
     </row>
     <row r="70" s="20" customFormat="1" spans="1:5">
       <c r="A70" s="27" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="B70" s="27"/>
       <c r="C70" s="27"/>
@@ -37260,7 +37328,7 @@
     </row>
     <row r="74" s="20" customFormat="1" spans="1:17">
       <c r="A74" s="21" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -37293,7 +37361,7 @@
         <v>1279</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="F75" s="10" t="s">
         <v>844</v>
@@ -37326,10 +37394,10 @@
         <v>852</v>
       </c>
       <c r="P75" s="10" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="Q75" s="10" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="76" s="20" customFormat="1" spans="1:17">
@@ -37346,43 +37414,43 @@
         <v>961</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="G76" s="11" t="s">
         <v>853</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="I76" s="33">
         <v>6456788899</v>
       </c>
       <c r="J76" s="26" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="K76" s="29" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="L76" s="11" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="M76" s="11" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="N76" s="29" t="s">
         <v>1036</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="P76" s="11" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="Q76" s="11" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="77" s="20" customFormat="1" spans="1:17">
@@ -37404,7 +37472,7 @@
     </row>
     <row r="78" s="20" customFormat="1" spans="1:17">
       <c r="A78" s="21" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
@@ -37490,7 +37558,7 @@
     </row>
     <row r="82" s="20" customFormat="1" spans="1:17">
       <c r="A82" s="27" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B82" s="27"/>
       <c r="C82" s="27"/>
@@ -37569,7 +37637,7 @@
     </row>
     <row r="86" s="20" customFormat="1" spans="1:17">
       <c r="A86" s="27" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="B86" s="27"/>
       <c r="C86" s="27"/>
@@ -37648,7 +37716,7 @@
     </row>
     <row r="90" s="20" customFormat="1" spans="1:17">
       <c r="A90" s="27" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
@@ -37713,7 +37781,7 @@
     </row>
     <row r="94" s="20" customFormat="1" spans="1:3">
       <c r="A94" s="21" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
@@ -37747,7 +37815,7 @@
     </row>
     <row r="98" s="20" customFormat="1" spans="1:3">
       <c r="A98" s="27" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="B98" s="27"/>
       <c r="C98" s="27"/>
@@ -37776,7 +37844,7 @@
     </row>
     <row r="102" s="20" customFormat="1" spans="1:3">
       <c r="A102" s="27" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="B102" s="27"/>
       <c r="C102" s="27"/>
@@ -37808,7 +37876,7 @@
     </row>
     <row r="106" s="20" customFormat="1" spans="1:3">
       <c r="A106" s="27" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
@@ -37840,7 +37908,7 @@
     </row>
     <row r="110" s="20" customFormat="1" spans="1:3">
       <c r="A110" s="27" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="B110" s="27"/>
       <c r="C110" s="27"/>
@@ -37872,7 +37940,7 @@
     </row>
     <row r="114" s="20" customFormat="1" spans="1:3">
       <c r="A114" s="27" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
@@ -37906,7 +37974,7 @@
     </row>
     <row r="118" s="20" customFormat="1" spans="1:3">
       <c r="A118" s="21" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="21"/>
@@ -37935,7 +38003,7 @@
     </row>
     <row r="122" s="20" customFormat="1" spans="1:3">
       <c r="A122" s="21" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="21"/>
@@ -37964,7 +38032,7 @@
     </row>
     <row r="126" s="20" customFormat="1" spans="1:3">
       <c r="A126" s="21" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
@@ -37993,7 +38061,7 @@
     </row>
     <row r="130" s="20" customFormat="1" spans="1:3">
       <c r="A130" s="27" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
@@ -38025,7 +38093,7 @@
     </row>
     <row r="134" s="20" customFormat="1" spans="1:3">
       <c r="A134" s="27" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
@@ -38057,7 +38125,7 @@
     </row>
     <row r="138" s="20" customFormat="1" spans="1:3">
       <c r="A138" s="27" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
@@ -38086,7 +38154,7 @@
     </row>
     <row r="142" s="20" customFormat="1" spans="1:3">
       <c r="A142" s="27" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
@@ -38115,7 +38183,7 @@
     </row>
     <row r="146" s="20" customFormat="1" spans="1:3">
       <c r="A146" s="27" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
@@ -38144,7 +38212,7 @@
     </row>
     <row r="150" s="20" customFormat="1" spans="1:3">
       <c r="A150" s="27" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
@@ -38173,7 +38241,7 @@
     </row>
     <row r="154" s="20" customFormat="1" spans="1:3">
       <c r="A154" s="27" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
@@ -38202,7 +38270,7 @@
     </row>
     <row r="158" s="20" customFormat="1" spans="1:3">
       <c r="A158" s="27" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
@@ -38231,7 +38299,7 @@
     </row>
     <row r="162" s="20" customFormat="1" spans="1:3">
       <c r="A162" s="27" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="B162" s="27"/>
       <c r="C162" s="27"/>
@@ -38260,7 +38328,7 @@
     </row>
     <row r="166" s="20" customFormat="1" spans="1:3">
       <c r="A166" s="27" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="B166" s="27"/>
       <c r="C166" s="27"/>
@@ -38289,7 +38357,7 @@
     </row>
     <row r="170" s="20" customFormat="1" spans="1:3">
       <c r="A170" s="27" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="B170" s="27"/>
       <c r="C170" s="27"/>
@@ -38318,7 +38386,7 @@
     </row>
     <row r="174" s="20" customFormat="1" spans="1:3">
       <c r="A174" s="27" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="B174" s="27"/>
       <c r="C174" s="27"/>
@@ -38347,7 +38415,7 @@
     </row>
     <row r="178" s="20" customFormat="1" spans="1:3">
       <c r="A178" s="27" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="B178" s="27"/>
       <c r="C178" s="27"/>
@@ -38376,7 +38444,7 @@
     </row>
     <row r="182" s="20" customFormat="1" spans="1:4">
       <c r="A182" s="21" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="B182" s="21"/>
       <c r="C182" s="21"/>
@@ -38412,7 +38480,7 @@
     </row>
     <row r="186" s="20" customFormat="1" spans="1:3">
       <c r="A186" s="27" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="B186" s="27"/>
       <c r="C186" s="27"/>
@@ -38441,7 +38509,7 @@
     </row>
     <row r="190" s="20" customFormat="1" spans="1:4">
       <c r="A190" s="27" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="B190" s="27"/>
       <c r="C190" s="27"/>
@@ -38477,7 +38545,7 @@
     </row>
     <row r="194" s="20" customFormat="1" spans="1:3">
       <c r="A194" s="27" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="B194" s="27"/>
       <c r="C194" s="27"/>
@@ -38506,7 +38574,7 @@
     </row>
     <row r="198" s="20" customFormat="1" spans="1:3">
       <c r="A198" s="27" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="B198" s="27"/>
       <c r="C198" s="27"/>
@@ -38535,7 +38603,7 @@
     </row>
     <row r="202" s="20" customFormat="1" spans="1:3">
       <c r="A202" s="27" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="B202" s="27"/>
       <c r="C202" s="27"/>
@@ -38999,7 +39067,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -39027,7 +39095,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -39055,7 +39123,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -39083,7 +39151,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -39111,7 +39179,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -39139,7 +39207,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -39167,7 +39235,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -39195,7 +39263,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -39223,7 +39291,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -39251,7 +39319,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -39279,7 +39347,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -39300,7 +39368,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>6</v>
@@ -39309,7 +39377,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -39382,7 +39450,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -39410,7 +39478,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -39438,7 +39506,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -39466,7 +39534,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -39494,7 +39562,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -39522,7 +39590,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -39532,34 +39600,34 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>542</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>4</v>
@@ -39576,28 +39644,28 @@
         <v>1282</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="H23" s="147" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="J23" s="147" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="K23" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>6</v>
@@ -39616,7 +39684,7 @@
     </row>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -39644,7 +39712,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -39672,7 +39740,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -39682,40 +39750,40 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>4</v>
@@ -39732,34 +39800,34 @@
         <v>1282</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H35" s="147" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="K35" s="147" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="L35" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>6</v>
@@ -39768,7 +39836,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -43702,7 +43770,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -43730,7 +43798,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -43758,7 +43826,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -43786,7 +43854,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -43814,7 +43882,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -43842,7 +43910,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -43870,7 +43938,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -43898,7 +43966,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -43926,7 +43994,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -43954,7 +44022,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -43982,7 +44050,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -44003,7 +44071,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>6</v>
@@ -44012,7 +44080,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -44082,7 +44150,7 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -44110,7 +44178,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" customFormat="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44138,7 +44206,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44166,7 +44234,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" customFormat="1" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44194,7 +44262,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" customFormat="1" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -44222,7 +44290,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -44232,34 +44300,34 @@
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>542</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>4</v>
@@ -44276,28 +44344,28 @@
         <v>1282</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H23" s="147" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="J23" s="147" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>6</v>
@@ -44316,7 +44384,7 @@
     </row>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -44344,7 +44412,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -44372,7 +44440,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -44382,40 +44450,40 @@
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>1168</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>4</v>
@@ -44432,34 +44500,34 @@
         <v>1282</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>853</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="H35" s="147" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>901</v>
       </c>
       <c r="K35" s="147" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>6</v>
@@ -44468,7 +44536,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" customFormat="1" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -44529,7 +44597,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -44557,7 +44625,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44585,7 +44653,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44613,7 +44681,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44641,7 +44709,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -44669,7 +44737,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -44697,7 +44765,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -44725,7 +44793,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -44753,7 +44821,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -44781,7 +44849,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -44809,7 +44877,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -44871,7 +44939,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -44899,7 +44967,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -44927,7 +44995,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -44955,7 +45023,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -44983,7 +45051,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -45011,7 +45079,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -45039,7 +45107,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -45067,7 +45135,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -45095,7 +45163,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -45123,7 +45191,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -45151,7 +45219,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -45213,7 +45281,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45241,7 +45309,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -45269,7 +45337,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -45297,7 +45365,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -45325,7 +45393,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -45353,7 +45421,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -45381,7 +45449,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -45409,7 +45477,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -45437,7 +45505,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -45465,7 +45533,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2059</v>
+        <v>2060</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -45493,7 +45561,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -45521,7 +45589,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -45549,7 +45617,7 @@
     <row r="48" customFormat="1"/>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>2062</v>
+        <v>2063</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -45577,7 +45645,7 @@
     <row r="52" customFormat="1"/>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -45605,7 +45673,7 @@
     <row r="56" customFormat="1"/>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>2064</v>
+        <v>2065</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -45633,7 +45701,7 @@
     <row r="60" customFormat="1"/>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -45661,7 +45729,7 @@
     <row r="64" customFormat="1"/>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -45689,7 +45757,7 @@
     <row r="68" customFormat="1"/>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>2067</v>
+        <v>2068</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -45717,7 +45785,7 @@
     <row r="72" customFormat="1"/>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>2068</v>
+        <v>2069</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -45745,7 +45813,7 @@
     <row r="76" customFormat="1"/>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>2069</v>
+        <v>2070</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -45773,7 +45841,7 @@
     <row r="80" customFormat="1"/>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -45801,7 +45869,7 @@
     <row r="84" customFormat="1"/>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>2071</v>
+        <v>2072</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -45828,7 +45896,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -45902,7 +45970,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45930,7 +45998,7 @@
     <row r="4" customFormat="1"/>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -45958,7 +46026,7 @@
     <row r="8" customFormat="1"/>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>2075</v>
+        <v>2076</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -45986,7 +46054,7 @@
     <row r="12" customFormat="1"/>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>2076</v>
+        <v>2077</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -46014,7 +46082,7 @@
     <row r="16" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>2077</v>
+        <v>2078</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -46042,7 +46110,7 @@
     <row r="20" customFormat="1"/>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>2078</v>
+        <v>2079</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -46070,7 +46138,7 @@
     <row r="24" customFormat="1"/>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>2079</v>
+        <v>2080</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -46098,7 +46166,7 @@
     <row r="28" customFormat="1"/>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>2080</v>
+        <v>2081</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -46126,7 +46194,7 @@
     <row r="32" customFormat="1"/>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>2081</v>
+        <v>2082</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -46154,7 +46222,7 @@
     <row r="36" customFormat="1"/>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>2082</v>
+        <v>2083</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -46182,7 +46250,7 @@
     <row r="40" customFormat="1"/>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -46210,7 +46278,7 @@
     <row r="44" customFormat="1"/>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -46238,7 +46306,7 @@
     <row r="48" customFormat="1"/>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>2085</v>
+        <v>2086</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -46266,7 +46334,7 @@
     <row r="52" customFormat="1"/>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -46294,7 +46362,7 @@
     <row r="56" customFormat="1"/>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>2087</v>
+        <v>2088</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -46322,7 +46390,7 @@
     <row r="60" customFormat="1"/>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>2088</v>
+        <v>2089</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -46350,7 +46418,7 @@
     <row r="64" customFormat="1"/>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>2089</v>
+        <v>2090</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -46378,7 +46446,7 @@
     <row r="68" customFormat="1"/>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -46406,7 +46474,7 @@
     <row r="72" customFormat="1"/>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -46434,7 +46502,7 @@
     <row r="76" customFormat="1"/>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -46462,7 +46530,7 @@
     <row r="80" customFormat="1"/>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -46490,7 +46558,7 @@
     <row r="84" customFormat="1"/>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>2094</v>
+        <v>2095</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -46518,7 +46586,7 @@
     <row r="88" customFormat="1"/>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>2095</v>
+        <v>2096</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>

</xml_diff>

<commit_message>
Added XP8_phonedailer module with supporting modules
</commit_message>
<xml_diff>
--- a/src/test/resources/documents/XP5S_All_TC.xlsx
+++ b/src/test/resources/documents/XP5S_All_TC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8355" tabRatio="656" firstSheet="20" activeTab="26"/>
+    <workbookView windowWidth="20385" windowHeight="8355" tabRatio="656" firstSheet="22" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,15 @@
     <sheet name="XP5S_SonimCare" sheetId="25" r:id="rId25"/>
     <sheet name="XP8_ContactTransfer" sheetId="26" r:id="rId26"/>
     <sheet name="XP8_SafeGuard" sheetId="27" r:id="rId27"/>
+    <sheet name="XP8_PhoneDialer_new" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <oleSize ref="A10:F60"/>
+  <oleSize ref="A13:F63"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135">
   <si>
     <t>Sonimcare</t>
   </si>
@@ -6413,6 +6414,51 @@
   </si>
   <si>
     <t>XP8_TC_011_SG_Validate_Application_PIN_Timeout</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_001_Validate_Phone_Application_Launch</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_002_Validate_Phone_App_Home_Page_Without_call_Log</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_003_Validate_Make_A_Call</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_004_Save_contact_from_phone_dialer</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>+919876543210</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_005_Validate_favourite_or_frequent_contact_list</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_006_Validate_Search_option</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_007_Validate_Send_SMS_from_recent_call_Log</t>
+  </si>
+  <si>
+    <t>Automation message</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_008_Validate_Add_New_Contact</t>
+  </si>
+  <si>
+    <t>9876543201</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>9686868686</t>
+  </si>
+  <si>
+    <t>XP8_PhoneDialer_009_Validate_Call_blocking_and_unblocking_functionality</t>
   </si>
 </sst>
 </file>
@@ -6420,10 +6466,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -6502,24 +6548,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6527,14 +6558,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6557,7 +6580,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6572,29 +6647,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6610,14 +6663,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6698,19 +6744,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6728,13 +6804,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6746,7 +6822,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6758,49 +6864,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6812,67 +6912,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6983,27 +7029,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7051,16 +7086,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7079,151 +7114,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -26690,8 +26736,8 @@
   <sheetPr/>
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -47091,8 +47137,8 @@
   <sheetPr/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -47422,6 +47468,324 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A41:C41"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="30.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="45.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="17.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="11.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" customFormat="1" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1"/>
+    <row r="5" customFormat="1" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>2121</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="1" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:3">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>2122</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" customFormat="1" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:3">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1"/>
+    <row r="13" customFormat="1" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>2123</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2124</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" ht="17" customHeight="1" spans="1:5">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D15" s="147" t="s">
+        <v>2125</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1"/>
+    <row r="17" customFormat="1" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>2126</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" customFormat="1" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" spans="1:3">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1"/>
+    <row r="21" customFormat="1" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>2127</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" customFormat="1" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" spans="1:3">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1"/>
+    <row r="25" customFormat="1" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" customFormat="1" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" spans="1:3">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1"/>
+    <row r="29" customFormat="1" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="147" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D31" s="147" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" customFormat="1"/>
+    <row r="33" customFormat="1" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>2134</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" customFormat="1" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" customFormat="1" spans="1:3">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A33:C33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>